<commit_message>
fixed small bugs in plotting, version 1.0.7
</commit_message>
<xml_diff>
--- a/docs/Examples/Cpx_Cpx_Liq_Thermobarometry/Cpx_Liq_Example.xlsx
+++ b/docs/Examples/Cpx_Cpx_Liq_Thermobarometry/Cpx_Liq_Example.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\penny\OneDrive - Oregon State University\Postdoc\PyMME\MyBarometers\Thermobar_outer\Examples\Cpx_Cpx_Liq_Thermobarometry\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Postdoc\PyMME\MyBarometers\Thermobar_outer\docs\Examples\Cpx_Cpx_Liq_Thermobarometry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A85E6BE-4D91-4C32-8F38-DD0B56FA1EA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A654CE-6F73-41C4-98DF-17F2714B222E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{E8E7985B-3CF2-4EFE-9D4B-8895F7D277F0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" xr2:uid="{E8E7985B-3CF2-4EFE-9D4B-8895F7D277F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" iterateCount="500"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="60">
   <si>
     <t>Sample_ID</t>
   </si>
@@ -173,6 +173,48 @@
   </si>
   <si>
     <t>Cr2O3_cpx</t>
+  </si>
+  <si>
+    <t>Test3</t>
+  </si>
+  <si>
+    <t>Test4</t>
+  </si>
+  <si>
+    <t>Test5</t>
+  </si>
+  <si>
+    <t>Test6</t>
+  </si>
+  <si>
+    <t>Test7</t>
+  </si>
+  <si>
+    <t>Test8</t>
+  </si>
+  <si>
+    <t>Test9</t>
+  </si>
+  <si>
+    <t>Test10</t>
+  </si>
+  <si>
+    <t>Test11</t>
+  </si>
+  <si>
+    <t>Test14</t>
+  </si>
+  <si>
+    <t>Test15</t>
+  </si>
+  <si>
+    <t>Test16</t>
+  </si>
+  <si>
+    <t>Test17</t>
+  </si>
+  <si>
+    <t>index</t>
   </si>
 </sst>
 </file>
@@ -182,7 +224,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,8 +250,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -228,6 +276,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -241,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -267,6 +321,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,442 +636,1573 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E477760D-8872-44D0-99F1-C56BCECBE94C}">
-  <dimension ref="A1:W6"/>
+  <dimension ref="A1:X21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.33203125" customWidth="1"/>
+    <col min="1" max="2" width="39.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6">
         <v>51.1</v>
       </c>
-      <c r="C2" s="6">
+      <c r="D2" s="6">
         <v>0.93</v>
       </c>
-      <c r="D2" s="6">
+      <c r="E2" s="6">
         <v>17.5</v>
       </c>
-      <c r="E2" s="6">
+      <c r="F2" s="6">
         <v>8.91</v>
       </c>
-      <c r="F2" s="6">
+      <c r="G2" s="6">
         <v>0.18</v>
       </c>
-      <c r="G2" s="7">
+      <c r="H2" s="7">
         <v>6.09</v>
       </c>
-      <c r="H2" s="6">
+      <c r="I2" s="6">
         <v>11.5</v>
       </c>
-      <c r="I2" s="6">
+      <c r="J2" s="6">
         <v>3.53</v>
       </c>
-      <c r="J2" s="6">
+      <c r="K2" s="6">
         <v>0.17</v>
       </c>
-      <c r="K2" s="6">
+      <c r="L2" s="6">
         <v>0</v>
       </c>
-      <c r="L2" s="6">
+      <c r="M2" s="6">
         <v>0.15</v>
       </c>
-      <c r="M2" s="6">
+      <c r="N2" s="6">
         <v>3.8</v>
       </c>
-      <c r="N2" s="8">
+      <c r="O2" s="8">
         <v>51.5</v>
       </c>
-      <c r="O2" s="8">
+      <c r="P2" s="8">
         <v>0.5</v>
       </c>
-      <c r="P2" s="8">
+      <c r="Q2" s="8">
         <v>3.7</v>
       </c>
-      <c r="Q2" s="8">
+      <c r="R2" s="8">
         <v>5.18</v>
       </c>
-      <c r="R2" s="8">
+      <c r="S2" s="8">
         <v>0.09</v>
       </c>
-      <c r="S2" s="8">
+      <c r="T2" s="8">
         <v>15.8</v>
       </c>
-      <c r="T2" s="8">
+      <c r="U2" s="8">
         <v>22.8</v>
       </c>
-      <c r="U2" s="8">
+      <c r="V2" s="8">
         <v>0.24</v>
       </c>
-      <c r="V2" s="8">
+      <c r="W2" s="8">
         <v>0</v>
       </c>
-      <c r="W2" s="8">
+      <c r="X2" s="8">
         <v>0.66</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6">
         <v>51.5</v>
       </c>
-      <c r="C3" s="6">
+      <c r="D3" s="6">
         <v>1.19</v>
       </c>
-      <c r="D3" s="6">
+      <c r="E3" s="6">
         <v>19.2</v>
       </c>
-      <c r="E3" s="6">
+      <c r="F3" s="6">
         <v>8.6999999999999993</v>
       </c>
-      <c r="F3" s="6">
+      <c r="G3" s="6">
         <v>0.19</v>
       </c>
-      <c r="G3" s="7">
+      <c r="H3" s="7">
         <v>4.9800000000000004</v>
       </c>
-      <c r="H3" s="6">
+      <c r="I3" s="6">
         <v>10</v>
       </c>
-      <c r="I3" s="6">
+      <c r="J3" s="6">
         <v>3.72</v>
       </c>
-      <c r="J3" s="6">
+      <c r="K3" s="6">
         <v>0.42</v>
       </c>
-      <c r="K3" s="6">
+      <c r="L3" s="6">
         <v>0</v>
       </c>
-      <c r="L3" s="6">
+      <c r="M3" s="6">
         <v>0.14000000000000001</v>
       </c>
-      <c r="M3" s="6">
+      <c r="N3" s="6">
         <v>6.2</v>
       </c>
-      <c r="N3" s="8">
+      <c r="O3" s="8">
         <v>50.3</v>
       </c>
-      <c r="O3" s="8">
+      <c r="P3" s="8">
         <v>0.73</v>
       </c>
-      <c r="P3" s="8">
+      <c r="Q3" s="8">
         <v>4.12</v>
       </c>
-      <c r="Q3" s="8">
+      <c r="R3" s="8">
         <v>5.83</v>
       </c>
-      <c r="R3" s="8">
+      <c r="S3" s="8">
         <v>0</v>
       </c>
-      <c r="S3" s="8">
+      <c r="T3" s="8">
         <v>15</v>
       </c>
-      <c r="T3" s="8">
+      <c r="U3" s="8">
         <v>22.7</v>
       </c>
-      <c r="U3" s="8">
+      <c r="V3" s="8">
         <v>0.24</v>
       </c>
-      <c r="V3" s="8">
+      <c r="W3" s="8">
         <v>0</v>
       </c>
-      <c r="W3" s="8">
+      <c r="X3" s="8">
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="6">
         <v>59.1</v>
       </c>
-      <c r="C4" s="6">
+      <c r="D4" s="6">
         <v>0.54</v>
       </c>
-      <c r="D4" s="6">
+      <c r="E4" s="6">
         <v>19.100000000000001</v>
       </c>
-      <c r="E4" s="6">
+      <c r="F4" s="6">
         <v>5.22</v>
       </c>
-      <c r="F4" s="6">
+      <c r="G4" s="6">
         <v>0.19</v>
       </c>
-      <c r="G4" s="7">
+      <c r="H4" s="7">
         <v>3.25</v>
       </c>
-      <c r="H4" s="6">
+      <c r="I4" s="6">
         <v>7.45</v>
       </c>
-      <c r="I4" s="6">
+      <c r="J4" s="6">
         <v>4</v>
       </c>
-      <c r="J4" s="6">
+      <c r="K4" s="6">
         <v>0.88</v>
       </c>
-      <c r="K4" s="6">
+      <c r="L4" s="6">
         <v>0</v>
       </c>
-      <c r="L4" s="6">
+      <c r="M4" s="6">
         <v>0.31</v>
       </c>
-      <c r="M4" s="6">
+      <c r="N4" s="6">
         <v>6.2</v>
       </c>
-      <c r="N4" s="8">
+      <c r="O4" s="8">
         <v>47.3</v>
       </c>
-      <c r="O4" s="8">
+      <c r="P4" s="8">
         <v>1.75</v>
       </c>
-      <c r="P4" s="8">
+      <c r="Q4" s="8">
         <v>7.85</v>
       </c>
-      <c r="Q4" s="8">
+      <c r="R4" s="8">
         <v>6.51</v>
       </c>
-      <c r="R4" s="8">
+      <c r="S4" s="8">
         <v>0.14000000000000001</v>
       </c>
-      <c r="S4" s="8">
+      <c r="T4" s="8">
         <v>13.1</v>
       </c>
-      <c r="T4" s="8">
+      <c r="U4" s="8">
         <v>22.5</v>
       </c>
-      <c r="U4" s="8">
+      <c r="V4" s="8">
         <v>0.25</v>
       </c>
-      <c r="V4" s="8">
+      <c r="W4" s="8">
         <v>0</v>
       </c>
-      <c r="W4" s="8">
+      <c r="X4" s="8">
         <v>0.22</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" s="6">
         <v>52.5</v>
       </c>
-      <c r="C5" s="6">
+      <c r="D5" s="6">
         <v>0.98</v>
       </c>
-      <c r="D5" s="6">
+      <c r="E5" s="6">
         <v>19.2</v>
       </c>
-      <c r="E5" s="6">
+      <c r="F5" s="6">
         <v>8.0399999999999991</v>
       </c>
-      <c r="F5" s="6">
+      <c r="G5" s="6">
         <v>0.2</v>
       </c>
-      <c r="G5" s="7">
+      <c r="H5" s="7">
         <v>4.99</v>
       </c>
-      <c r="H5" s="6">
+      <c r="I5" s="6">
         <v>9.64</v>
       </c>
-      <c r="I5" s="6">
+      <c r="J5" s="6">
         <v>4.1500000000000004</v>
       </c>
-      <c r="J5" s="6">
+      <c r="K5" s="6">
         <v>0.21</v>
       </c>
-      <c r="K5" s="6">
+      <c r="L5" s="6">
         <v>0</v>
       </c>
-      <c r="L5" s="6">
+      <c r="M5" s="6">
         <v>0.14000000000000001</v>
       </c>
-      <c r="M5" s="6">
+      <c r="N5" s="6">
         <v>6.2</v>
       </c>
-      <c r="N5" s="8">
+      <c r="O5" s="8">
         <v>51.1</v>
       </c>
-      <c r="O5" s="8">
+      <c r="P5" s="8">
         <v>0.63</v>
       </c>
-      <c r="P5" s="8">
+      <c r="Q5" s="8">
         <v>4.41</v>
       </c>
-      <c r="Q5" s="8">
+      <c r="R5" s="8">
         <v>5.66</v>
       </c>
-      <c r="R5" s="8">
+      <c r="S5" s="8">
         <v>0.13</v>
       </c>
-      <c r="S5" s="8">
+      <c r="T5" s="8">
         <v>15.6</v>
       </c>
-      <c r="T5" s="8">
+      <c r="U5" s="8">
         <v>22.6</v>
       </c>
-      <c r="U5" s="8">
+      <c r="V5" s="8">
         <v>0.23</v>
       </c>
-      <c r="V5" s="8">
+      <c r="W5" s="8">
         <v>0</v>
       </c>
-      <c r="W5" s="8">
+      <c r="X5" s="8">
         <v>0.27</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" s="6">
         <v>56.2</v>
       </c>
-      <c r="C6" s="6">
+      <c r="D6" s="6">
         <v>0.34</v>
       </c>
-      <c r="D6" s="6">
+      <c r="E6" s="6">
         <v>20.399999999999999</v>
       </c>
-      <c r="E6" s="6">
+      <c r="F6" s="6">
         <v>5.88</v>
       </c>
-      <c r="F6" s="6">
+      <c r="G6" s="6">
         <v>0.2</v>
       </c>
-      <c r="G6" s="7">
+      <c r="H6" s="7">
         <v>2.58</v>
       </c>
-      <c r="H6" s="6">
+      <c r="I6" s="6">
         <v>7.18</v>
       </c>
-      <c r="I6" s="6">
+      <c r="J6" s="6">
         <v>6.02</v>
       </c>
-      <c r="J6" s="6">
+      <c r="K6" s="6">
         <v>1.02</v>
       </c>
-      <c r="K6" s="6">
+      <c r="L6" s="6">
         <v>0</v>
       </c>
-      <c r="L6" s="6">
+      <c r="M6" s="6">
         <v>0.23</v>
       </c>
-      <c r="M6" s="6">
+      <c r="N6" s="6">
         <v>6.2</v>
       </c>
-      <c r="N6" s="8">
+      <c r="O6" s="8">
         <v>51</v>
       </c>
-      <c r="O6" s="8">
+      <c r="P6" s="8">
         <v>0.56000000000000005</v>
       </c>
-      <c r="P6" s="8">
+      <c r="Q6" s="8">
         <v>4.1399999999999997</v>
       </c>
-      <c r="Q6" s="8">
+      <c r="R6" s="8">
         <v>7.33</v>
       </c>
-      <c r="R6" s="8">
+      <c r="S6" s="8">
         <v>0.2</v>
       </c>
-      <c r="S6" s="8">
+      <c r="T6" s="8">
         <v>14.4</v>
       </c>
-      <c r="T6" s="8">
+      <c r="U6" s="8">
         <v>22.4</v>
       </c>
-      <c r="U6" s="8">
+      <c r="V6" s="8">
         <v>0.31</v>
       </c>
-      <c r="V6" s="8">
+      <c r="W6" s="8">
         <v>0</v>
       </c>
-      <c r="W6" s="8">
+      <c r="X6" s="8">
         <v>0.09</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="9">
+        <v>5</v>
+      </c>
+      <c r="C7" s="9">
+        <v>51.865718442961551</v>
+      </c>
+      <c r="D7" s="9">
+        <v>1.2673398711663131</v>
+      </c>
+      <c r="E7" s="9">
+        <v>18.497538715262095</v>
+      </c>
+      <c r="F7" s="9">
+        <v>9.335870758456128</v>
+      </c>
+      <c r="G7" s="9">
+        <v>1.0026088268711173</v>
+      </c>
+      <c r="H7" s="9">
+        <v>6.8197882556432887</v>
+      </c>
+      <c r="I7" s="9">
+        <v>11.510631257075989</v>
+      </c>
+      <c r="J7" s="9">
+        <v>4.5236118223563526</v>
+      </c>
+      <c r="K7" s="9">
+        <v>0.72525785581109359</v>
+      </c>
+      <c r="L7" s="9">
+        <v>0.61797074487623782</v>
+      </c>
+      <c r="M7" s="9">
+        <v>0.92651082175509591</v>
+      </c>
+      <c r="N7" s="9">
+        <v>4.315351543256476</v>
+      </c>
+      <c r="O7" s="9">
+        <v>51.893554315312223</v>
+      </c>
+      <c r="P7" s="9">
+        <v>0.98564789982641987</v>
+      </c>
+      <c r="Q7" s="9">
+        <v>4.3740390004201855</v>
+      </c>
+      <c r="R7" s="9">
+        <v>6.0147743287412174</v>
+      </c>
+      <c r="S7" s="9">
+        <v>0.42703725719958097</v>
+      </c>
+      <c r="T7" s="9">
+        <v>15.882719032522116</v>
+      </c>
+      <c r="U7" s="9">
+        <v>23.735223843272621</v>
+      </c>
+      <c r="V7" s="9">
+        <v>0.64098873498527209</v>
+      </c>
+      <c r="W7" s="9">
+        <v>0.21431101552434106</v>
+      </c>
+      <c r="X7" s="9">
+        <v>1.476324925244453</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>51.886153736234832</v>
+      </c>
+      <c r="D8">
+        <v>1.3567543480795661</v>
+      </c>
+      <c r="E8">
+        <v>17.961255051067532</v>
+      </c>
+      <c r="F8">
+        <v>9.020532645782037</v>
+      </c>
+      <c r="G8">
+        <v>0.50395815308879288</v>
+      </c>
+      <c r="H8">
+        <v>6.3678123338073069</v>
+      </c>
+      <c r="I8">
+        <v>12.150022261322444</v>
+      </c>
+      <c r="J8">
+        <v>3.5759186586304454</v>
+      </c>
+      <c r="K8">
+        <v>1.0979322882766491</v>
+      </c>
+      <c r="L8">
+        <v>0.37755022670730842</v>
+      </c>
+      <c r="M8">
+        <v>0.57040601361118448</v>
+      </c>
+      <c r="N8">
+        <v>3.8187589261275554</v>
+      </c>
+      <c r="O8">
+        <v>51.671503192945664</v>
+      </c>
+      <c r="P8">
+        <v>1.222254136090335</v>
+      </c>
+      <c r="Q8">
+        <v>4.4246093292211359</v>
+      </c>
+      <c r="R8">
+        <v>5.7550141673962214</v>
+      </c>
+      <c r="S8">
+        <v>0.53748341673628042</v>
+      </c>
+      <c r="T8">
+        <v>15.849673025564531</v>
+      </c>
+      <c r="U8">
+        <v>23.601948250038561</v>
+      </c>
+      <c r="V8">
+        <v>0.5630639163927007</v>
+      </c>
+      <c r="W8">
+        <v>0.14998362434199963</v>
+      </c>
+      <c r="X8">
+        <v>1.4601156133221038</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>51.496827475661696</v>
+      </c>
+      <c r="D9">
+        <v>0.95859336354547375</v>
+      </c>
+      <c r="E9">
+        <v>17.847817331587667</v>
+      </c>
+      <c r="F9">
+        <v>9.7834654417587448</v>
+      </c>
+      <c r="G9">
+        <v>0.68499895439856329</v>
+      </c>
+      <c r="H9">
+        <v>6.1664901338296119</v>
+      </c>
+      <c r="I9">
+        <v>12.123362283370151</v>
+      </c>
+      <c r="J9">
+        <v>4.1724487024585901</v>
+      </c>
+      <c r="K9">
+        <v>0.42682496868970898</v>
+      </c>
+      <c r="L9">
+        <v>0.40629586545009744</v>
+      </c>
+      <c r="M9">
+        <v>1.0025932911675357</v>
+      </c>
+      <c r="N9">
+        <v>4.5551681484457864</v>
+      </c>
+      <c r="O9">
+        <v>52.462670991812608</v>
+      </c>
+      <c r="P9">
+        <v>0.86136591024308318</v>
+      </c>
+      <c r="Q9">
+        <v>4.3064557449076917</v>
+      </c>
+      <c r="R9">
+        <v>5.5215737872049386</v>
+      </c>
+      <c r="S9">
+        <v>9.34050860834508E-2</v>
+      </c>
+      <c r="T9">
+        <v>15.93172065600292</v>
+      </c>
+      <c r="U9">
+        <v>22.890466836018312</v>
+      </c>
+      <c r="V9">
+        <v>0.83925573351594551</v>
+      </c>
+      <c r="W9">
+        <v>0.82914118616813537</v>
+      </c>
+      <c r="X9">
+        <v>1.605553232707617</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>51.570401867075915</v>
+      </c>
+      <c r="D10">
+        <v>1.5870710689973315</v>
+      </c>
+      <c r="E10">
+        <v>18.282228805852505</v>
+      </c>
+      <c r="F10">
+        <v>9.614433985390999</v>
+      </c>
+      <c r="G10">
+        <v>1.1535720612564788</v>
+      </c>
+      <c r="H10">
+        <v>6.8966177195360805</v>
+      </c>
+      <c r="I10">
+        <v>12.43688792476399</v>
+      </c>
+      <c r="J10">
+        <v>3.6383022554019151</v>
+      </c>
+      <c r="K10">
+        <v>0.31964387617326651</v>
+      </c>
+      <c r="L10">
+        <v>3.5171387976879465E-2</v>
+      </c>
+      <c r="M10">
+        <v>0.67016353681557705</v>
+      </c>
+      <c r="N10">
+        <v>4.3256449098772087</v>
+      </c>
+      <c r="O10">
+        <v>52.341465226980908</v>
+      </c>
+      <c r="P10">
+        <v>0.55852050587880908</v>
+      </c>
+      <c r="Q10">
+        <v>4.3325191641093754</v>
+      </c>
+      <c r="R10">
+        <v>5.3072896406974497</v>
+      </c>
+      <c r="S10">
+        <v>0.53140757013931128</v>
+      </c>
+      <c r="T10">
+        <v>16.743678047328221</v>
+      </c>
+      <c r="U10">
+        <v>22.820816486065258</v>
+      </c>
+      <c r="V10">
+        <v>0.35614767019017946</v>
+      </c>
+      <c r="W10">
+        <v>0.15144664943976338</v>
+      </c>
+      <c r="X10">
+        <v>1.3282328697202099</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>51.439834171071247</v>
+      </c>
+      <c r="D11">
+        <v>1.4451195848705416</v>
+      </c>
+      <c r="E11">
+        <v>18.27756091498037</v>
+      </c>
+      <c r="F11">
+        <v>9.3680601190492609</v>
+      </c>
+      <c r="G11">
+        <v>0.55552482742864329</v>
+      </c>
+      <c r="H11">
+        <v>6.6493279993038481</v>
+      </c>
+      <c r="I11">
+        <v>11.852626648439049</v>
+      </c>
+      <c r="J11">
+        <v>4.1458047810088372</v>
+      </c>
+      <c r="K11">
+        <v>0.27730263348001638</v>
+      </c>
+      <c r="L11">
+        <v>6.3636605598579976E-2</v>
+      </c>
+      <c r="M11">
+        <v>0.96678131857867622</v>
+      </c>
+      <c r="N11">
+        <v>4.2504030371292263</v>
+      </c>
+      <c r="O11">
+        <v>51.905733329480441</v>
+      </c>
+      <c r="P11">
+        <v>0.64309690114219376</v>
+      </c>
+      <c r="Q11">
+        <v>3.8801632600366798</v>
+      </c>
+      <c r="R11">
+        <v>5.6518302849248174</v>
+      </c>
+      <c r="S11">
+        <v>0.61460641296147256</v>
+      </c>
+      <c r="T11">
+        <v>16.14641515087272</v>
+      </c>
+      <c r="U11">
+        <v>23.347920821527815</v>
+      </c>
+      <c r="V11">
+        <v>0.63320293760494617</v>
+      </c>
+      <c r="W11">
+        <v>0.7615388621871495</v>
+      </c>
+      <c r="X11">
+        <v>1.0275089138205837</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>51.569363372340959</v>
+      </c>
+      <c r="D12">
+        <v>1.0266673967320137</v>
+      </c>
+      <c r="E12">
+        <v>18.128996643102507</v>
+      </c>
+      <c r="F12">
+        <v>9.0306815164663643</v>
+      </c>
+      <c r="G12">
+        <v>0.42374875712699039</v>
+      </c>
+      <c r="H12">
+        <v>7.0575291219161036</v>
+      </c>
+      <c r="I12">
+        <v>11.952309297935246</v>
+      </c>
+      <c r="J12">
+        <v>3.7516724011044991</v>
+      </c>
+      <c r="K12">
+        <v>0.48014711395077314</v>
+      </c>
+      <c r="L12">
+        <v>0.98137316480940051</v>
+      </c>
+      <c r="M12">
+        <v>0.28217134971775681</v>
+      </c>
+      <c r="N12">
+        <v>3.9497695101041908</v>
+      </c>
+      <c r="O12">
+        <v>51.705545145442507</v>
+      </c>
+      <c r="P12">
+        <v>0.69744360186242083</v>
+      </c>
+      <c r="Q12">
+        <v>4.4061958174098743</v>
+      </c>
+      <c r="R12">
+        <v>5.7461365018638393</v>
+      </c>
+      <c r="S12">
+        <v>0.44383151173518653</v>
+      </c>
+      <c r="T12">
+        <v>15.907584862494522</v>
+      </c>
+      <c r="U12">
+        <v>23.482414605674716</v>
+      </c>
+      <c r="V12">
+        <v>1.1757276681180988</v>
+      </c>
+      <c r="W12">
+        <v>0.57197331573894405</v>
+      </c>
+      <c r="X12">
+        <v>1.486150631651753</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>51.891533338037682</v>
+      </c>
+      <c r="D13">
+        <v>1.0565977590274738</v>
+      </c>
+      <c r="E13">
+        <v>18.446561665071453</v>
+      </c>
+      <c r="F13">
+        <v>9.2129910500088297</v>
+      </c>
+      <c r="G13">
+        <v>0.23401712237681777</v>
+      </c>
+      <c r="H13">
+        <v>6.5571215866313741</v>
+      </c>
+      <c r="I13">
+        <v>12.269853462913524</v>
+      </c>
+      <c r="J13">
+        <v>3.9588722622861243</v>
+      </c>
+      <c r="K13">
+        <v>0.5447821032181478</v>
+      </c>
+      <c r="L13">
+        <v>4.2744582562208255E-2</v>
+      </c>
+      <c r="M13">
+        <v>0.86729760428430525</v>
+      </c>
+      <c r="N13">
+        <v>4.5271540781189685</v>
+      </c>
+      <c r="O13">
+        <v>52.200290820094978</v>
+      </c>
+      <c r="P13">
+        <v>1.4677591887478458</v>
+      </c>
+      <c r="Q13">
+        <v>4.0773998570820336</v>
+      </c>
+      <c r="R13">
+        <v>5.6073692277314144</v>
+      </c>
+      <c r="S13">
+        <v>0.83262604573184928</v>
+      </c>
+      <c r="T13">
+        <v>16.045590333276085</v>
+      </c>
+      <c r="U13">
+        <v>23.182284975249853</v>
+      </c>
+      <c r="V13">
+        <v>0.58793502600895886</v>
+      </c>
+      <c r="W13">
+        <v>0.62094267376136558</v>
+      </c>
+      <c r="X13">
+        <v>1.1704691372322329</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>51.926006931028162</v>
+      </c>
+      <c r="D14">
+        <v>1.4015043043948086</v>
+      </c>
+      <c r="E14">
+        <v>17.823167316460172</v>
+      </c>
+      <c r="F14">
+        <v>9.7827152503695842</v>
+      </c>
+      <c r="G14">
+        <v>0.57483404561247431</v>
+      </c>
+      <c r="H14">
+        <v>6.232652520705285</v>
+      </c>
+      <c r="I14">
+        <v>11.596630343227673</v>
+      </c>
+      <c r="J14">
+        <v>3.8852203067593551</v>
+      </c>
+      <c r="K14">
+        <v>1.0375493956737978</v>
+      </c>
+      <c r="L14">
+        <v>0.82167815515629983</v>
+      </c>
+      <c r="M14">
+        <v>0.68872182331471443</v>
+      </c>
+      <c r="N14">
+        <v>4.0448201461171003</v>
+      </c>
+      <c r="O14">
+        <v>51.725315498354846</v>
+      </c>
+      <c r="P14">
+        <v>0.74576138706968498</v>
+      </c>
+      <c r="Q14">
+        <v>4.5864852488463637</v>
+      </c>
+      <c r="R14">
+        <v>5.7367154523965151</v>
+      </c>
+      <c r="S14">
+        <v>0.55056075395631598</v>
+      </c>
+      <c r="T14">
+        <v>16.407622679469284</v>
+      </c>
+      <c r="U14">
+        <v>23.315816911051432</v>
+      </c>
+      <c r="V14">
+        <v>0.67503259304178176</v>
+      </c>
+      <c r="W14">
+        <v>0.81486542753760638</v>
+      </c>
+      <c r="X14">
+        <v>1.3493430335044079</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <v>51.45940222686783</v>
+      </c>
+      <c r="D15">
+        <v>1.0595341878629854</v>
+      </c>
+      <c r="E15">
+        <v>17.987605652532658</v>
+      </c>
+      <c r="F15">
+        <v>9.4619326816172222</v>
+      </c>
+      <c r="G15">
+        <v>0.90958596715161799</v>
+      </c>
+      <c r="H15">
+        <v>7.0128606614270232</v>
+      </c>
+      <c r="I15">
+        <v>12.439605000171683</v>
+      </c>
+      <c r="J15">
+        <v>4.4365027336377203</v>
+      </c>
+      <c r="K15">
+        <v>0.7642221343594755</v>
+      </c>
+      <c r="L15">
+        <v>0.24997598888778594</v>
+      </c>
+      <c r="M15">
+        <v>0.91187110533104376</v>
+      </c>
+      <c r="N15">
+        <v>3.876702655149376</v>
+      </c>
+      <c r="O15">
+        <v>51.892711139701696</v>
+      </c>
+      <c r="P15">
+        <v>0.91833503355131785</v>
+      </c>
+      <c r="Q15">
+        <v>3.8794929704930126</v>
+      </c>
+      <c r="R15">
+        <v>6.0017849451404324</v>
+      </c>
+      <c r="S15">
+        <v>0.22447557202237525</v>
+      </c>
+      <c r="T15">
+        <v>16.766704858640061</v>
+      </c>
+      <c r="U15">
+        <v>23.174609080930029</v>
+      </c>
+      <c r="V15">
+        <v>1.1067045592280014</v>
+      </c>
+      <c r="W15">
+        <v>0.54364809768301281</v>
+      </c>
+      <c r="X15">
+        <v>0.71977780946844006</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>51.45940222686783</v>
+      </c>
+      <c r="D16">
+        <v>1.0595341878629854</v>
+      </c>
+      <c r="E16">
+        <v>17.987605652532658</v>
+      </c>
+      <c r="F16">
+        <v>9.4619326816172222</v>
+      </c>
+      <c r="G16">
+        <v>0.90958596715161799</v>
+      </c>
+      <c r="H16">
+        <v>7.0128606614270232</v>
+      </c>
+      <c r="I16">
+        <v>12.439605000171683</v>
+      </c>
+      <c r="J16">
+        <v>4.4365027336377203</v>
+      </c>
+      <c r="K16">
+        <v>0.7642221343594755</v>
+      </c>
+      <c r="L16">
+        <v>0.24997598888778594</v>
+      </c>
+      <c r="M16">
+        <v>0.91187110533104376</v>
+      </c>
+      <c r="N16">
+        <v>3.876702655149376</v>
+      </c>
+      <c r="O16">
+        <v>51.892711139701696</v>
+      </c>
+      <c r="P16">
+        <v>0.91833503355131785</v>
+      </c>
+      <c r="Q16">
+        <v>3.8794929704930126</v>
+      </c>
+      <c r="R16">
+        <v>6.0017849451404324</v>
+      </c>
+      <c r="S16">
+        <v>0.22447557202237525</v>
+      </c>
+      <c r="T16">
+        <v>16.766704858640061</v>
+      </c>
+      <c r="U16">
+        <v>23.174609080930029</v>
+      </c>
+      <c r="V16">
+        <v>1.1067045592280014</v>
+      </c>
+      <c r="W16">
+        <v>0.54364809768301281</v>
+      </c>
+      <c r="X16">
+        <v>0.71977780946844006</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>51.45940222686783</v>
+      </c>
+      <c r="D17">
+        <v>1.0595341878629854</v>
+      </c>
+      <c r="E17">
+        <v>17.987605652532658</v>
+      </c>
+      <c r="F17">
+        <v>9.4619326816172222</v>
+      </c>
+      <c r="G17">
+        <v>0.90958596715161799</v>
+      </c>
+      <c r="H17">
+        <v>7.0128606614270232</v>
+      </c>
+      <c r="I17">
+        <v>12.439605000171683</v>
+      </c>
+      <c r="J17">
+        <v>4.4365027336377203</v>
+      </c>
+      <c r="K17">
+        <v>0.7642221343594755</v>
+      </c>
+      <c r="L17">
+        <v>0.24997598888778594</v>
+      </c>
+      <c r="M17">
+        <v>0.91187110533104376</v>
+      </c>
+      <c r="N17">
+        <v>3.876702655149376</v>
+      </c>
+      <c r="O17">
+        <v>51.892711139701696</v>
+      </c>
+      <c r="P17">
+        <v>0.91833503355131785</v>
+      </c>
+      <c r="Q17">
+        <v>3.8794929704930126</v>
+      </c>
+      <c r="R17">
+        <v>6.0017849451404324</v>
+      </c>
+      <c r="S17">
+        <v>0.22447557202237525</v>
+      </c>
+      <c r="T17">
+        <v>16.766704858640061</v>
+      </c>
+      <c r="U17">
+        <v>23.174609080930029</v>
+      </c>
+      <c r="V17">
+        <v>1.1067045592280014</v>
+      </c>
+      <c r="W17">
+        <v>0.54364809768301281</v>
+      </c>
+      <c r="X17">
+        <v>0.71977780946844006</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <v>51.473516189843437</v>
+      </c>
+      <c r="D18">
+        <v>1.1916600288481476</v>
+      </c>
+      <c r="E18">
+        <v>18.283674450401833</v>
+      </c>
+      <c r="F18">
+        <v>9.5424033262987233</v>
+      </c>
+      <c r="G18">
+        <v>1.0893982242076969</v>
+      </c>
+      <c r="H18">
+        <v>6.533626526151898</v>
+      </c>
+      <c r="I18">
+        <v>12.21939805251187</v>
+      </c>
+      <c r="J18">
+        <v>4.2370371491549452</v>
+      </c>
+      <c r="K18">
+        <v>0.94406118712758025</v>
+      </c>
+      <c r="L18">
+        <v>0.65231371306189512</v>
+      </c>
+      <c r="M18">
+        <v>0.64273843419040244</v>
+      </c>
+      <c r="N18">
+        <v>4.1919278016273704</v>
+      </c>
+      <c r="O18">
+        <v>52.006582092829838</v>
+      </c>
+      <c r="P18">
+        <v>1.4905628668765916</v>
+      </c>
+      <c r="Q18">
+        <v>4.6331486376500122</v>
+      </c>
+      <c r="R18">
+        <v>6.150715869156576</v>
+      </c>
+      <c r="S18">
+        <v>0.38396852599866638</v>
+      </c>
+      <c r="T18">
+        <v>15.82319277856905</v>
+      </c>
+      <c r="U18">
+        <v>23.08715665393159</v>
+      </c>
+      <c r="V18">
+        <v>1.171789048517673</v>
+      </c>
+      <c r="W18">
+        <v>0.58025771187647157</v>
+      </c>
+      <c r="X18">
+        <v>1.0727112256104308</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19">
+        <v>17</v>
+      </c>
+      <c r="C19">
+        <v>51.457640520181464</v>
+      </c>
+      <c r="D19">
+        <v>1.2926043804168008</v>
+      </c>
+      <c r="E19">
+        <v>18.492337209714769</v>
+      </c>
+      <c r="F19">
+        <v>9.4152698980543175</v>
+      </c>
+      <c r="G19">
+        <v>0.66776536095540462</v>
+      </c>
+      <c r="H19">
+        <v>6.7184713391011925</v>
+      </c>
+      <c r="I19">
+        <v>11.540913834012363</v>
+      </c>
+      <c r="J19">
+        <v>4.1237918180029887</v>
+      </c>
+      <c r="K19">
+        <v>1.0947576391992169</v>
+      </c>
+      <c r="L19">
+        <v>0.86709807760743696</v>
+      </c>
+      <c r="M19">
+        <v>0.75566906143731583</v>
+      </c>
+      <c r="N19">
+        <v>3.9832921334748832</v>
+      </c>
+      <c r="O19">
+        <v>51.986059192459578</v>
+      </c>
+      <c r="P19">
+        <v>1.1195478600134299</v>
+      </c>
+      <c r="Q19">
+        <v>4.1072575396856479</v>
+      </c>
+      <c r="R19">
+        <v>5.5875338322326051</v>
+      </c>
+      <c r="S19">
+        <v>0.86944749188414683</v>
+      </c>
+      <c r="T19">
+        <v>16.661903791152124</v>
+      </c>
+      <c r="U19">
+        <v>23.61611995637341</v>
+      </c>
+      <c r="V19">
+        <v>1.072979509659175</v>
+      </c>
+      <c r="W19">
+        <v>0.2427299533339542</v>
+      </c>
+      <c r="X19">
+        <v>1.0815947434012125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20">
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <v>51.62831641264259</v>
+      </c>
+      <c r="D20">
+        <v>1.6169337473284124</v>
+      </c>
+      <c r="E20">
+        <v>18.317892060947976</v>
+      </c>
+      <c r="F20">
+        <v>9.4955312666581335</v>
+      </c>
+      <c r="G20">
+        <v>1.0232414334561537</v>
+      </c>
+      <c r="H20">
+        <v>6.8262368557452628</v>
+      </c>
+      <c r="I20">
+        <v>12.14186690754463</v>
+      </c>
+      <c r="J20">
+        <v>4.0832273608493308</v>
+      </c>
+      <c r="K20">
+        <v>0.88192450254515198</v>
+      </c>
+      <c r="L20">
+        <v>0.43938251157895702</v>
+      </c>
+      <c r="M20">
+        <v>0.53949418830109452</v>
+      </c>
+      <c r="N20">
+        <v>4.6227918947504962</v>
+      </c>
+      <c r="O20">
+        <v>52.066982578091995</v>
+      </c>
+      <c r="P20">
+        <v>1.0701256846709648</v>
+      </c>
+      <c r="Q20">
+        <v>4.261571705299068</v>
+      </c>
+      <c r="R20">
+        <v>5.8452777504896281</v>
+      </c>
+      <c r="S20">
+        <v>0.27605664390567364</v>
+      </c>
+      <c r="T20">
+        <v>16.038722921259708</v>
+      </c>
+      <c r="U20">
+        <v>23.311110175801119</v>
+      </c>
+      <c r="V20">
+        <v>1.1263272099069428</v>
+      </c>
+      <c r="W20">
+        <v>0.11596958687622372</v>
+      </c>
+      <c r="X20">
+        <v>1.3906471195550267</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21">
+        <v>19</v>
+      </c>
+      <c r="C21">
+        <v>51.887171406111506</v>
+      </c>
+      <c r="D21">
+        <v>1.8393949438226582</v>
+      </c>
+      <c r="E21">
+        <v>18.139485768900666</v>
+      </c>
+      <c r="F21">
+        <v>9.5851814562849302</v>
+      </c>
+      <c r="G21">
+        <v>0.98432329629208049</v>
+      </c>
+      <c r="H21">
+        <v>7.0869217987317157</v>
+      </c>
+      <c r="I21">
+        <v>11.762257672470314</v>
+      </c>
+      <c r="J21">
+        <v>3.837002100853061</v>
+      </c>
+      <c r="K21">
+        <v>0.36098301204890637</v>
+      </c>
+      <c r="L21">
+        <v>0.61168868632447138</v>
+      </c>
+      <c r="M21">
+        <v>0.66610616168615411</v>
+      </c>
+      <c r="N21">
+        <v>3.9424997455787949</v>
+      </c>
+      <c r="O21">
+        <v>51.97389869641114</v>
+      </c>
+      <c r="P21">
+        <v>0.80967654122122568</v>
+      </c>
+      <c r="Q21">
+        <v>4.6656147897667513</v>
+      </c>
+      <c r="R21">
+        <v>5.8647178747404309</v>
+      </c>
+      <c r="S21">
+        <v>0.84025025380766305</v>
+      </c>
+      <c r="T21">
+        <v>16.467894112677506</v>
+      </c>
+      <c r="U21">
+        <v>23.319301569036305</v>
+      </c>
+      <c r="V21">
+        <v>0.87260685836650198</v>
+      </c>
+      <c r="W21">
+        <v>0.40434927829931155</v>
+      </c>
+      <c r="X21">
+        <v>0.94685742482012747</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1029,9 +2215,9 @@
       <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1102,7 +2288,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1173,7 +2359,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1244,7 +2430,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1315,7 +2501,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -1386,7 +2572,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>

</xml_diff>